<commit_message>
Se agrego demanda variable en el tiempo por sectores de consumo y se agrego base de datos con informacion util
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC92B7E-D267-471E-AB1D-717B18B41E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0B5EDE-E1E9-47A5-9FA2-ED0B9E5DF9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="3480" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3405" yWindow="3090" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>prueba_2040</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
+  <si>
+    <t>TOTAL_2040</t>
   </si>
 </sst>
 </file>
@@ -3315,10 +3321,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:H46"/>
+  <dimension ref="B3:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3557,12 +3563,12 @@
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G29" s="13"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="66" t="s">
         <v>103</v>
       </c>
@@ -3575,13 +3581,16 @@
       <c r="E35" s="66" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>105</v>
       </c>
@@ -3594,8 +3603,11 @@
       <c r="E37">
         <v>2019</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>105</v>
       </c>
@@ -3608,8 +3620,11 @@
       <c r="E38">
         <v>2020</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>105</v>
       </c>
@@ -3622,42 +3637,126 @@
       <c r="E39">
         <v>2023</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D40">
         <v>2025</v>
       </c>
       <c r="E40">
         <v>2025</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E41">
         <v>2027</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E42">
         <v>2030</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E43">
         <v>2033</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E44">
         <v>2035</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E45">
         <v>2037</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E46">
+        <v>2040</v>
+      </c>
+      <c r="F46">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58">
         <v>2040</v>
       </c>
     </row>
@@ -3674,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:F35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3750,6 +3849,20 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
     </row>
@@ -4184,7 +4297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se cargaron las dos refinerias
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0B5EDE-E1E9-47A5-9FA2-ED0B9E5DF9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA060EAE-C323-4944-B3E4-635A25103C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="3090" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>TOTAL_2040</t>
+  </si>
+  <si>
+    <t>UP, FX, LO</t>
   </si>
 </sst>
 </file>
@@ -1966,15 +1969,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2004,7 +2007,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="114300" y="1362075"/>
+          <a:off x="133350" y="1514475"/>
           <a:ext cx="6134100" cy="2943225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3323,7 +3326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F37" sqref="F37:F58"/>
     </sheetView>
   </sheetViews>
@@ -3773,8 +3776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3825,8 +3828,8 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>108</v>
+      <c r="B6" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>94</v>
@@ -3839,8 +3842,8 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>108</v>
+      <c r="B7" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>95</v>
@@ -3853,8 +3856,8 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>108</v>
+      <c r="B8" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
Se encontro el error de reservas, algunsa estan por encima de 2050
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA060EAE-C323-4944-B3E4-635A25103C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EE2C39-E1B2-40EC-BA9C-7D8B932F8C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="915" windowWidth="21600" windowHeight="11430" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="114">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>UP, FX, LO</t>
+  </si>
+  <si>
+    <t>prueba_2050</t>
   </si>
 </sst>
 </file>
@@ -3326,8 +3329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:F58"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3336,6 +3339,7 @@
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3566,12 +3570,12 @@
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G29" s="13"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="66" t="s">
         <v>103</v>
       </c>
@@ -3587,13 +3591,16 @@
       <c r="F35" s="66" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>105</v>
       </c>
@@ -3609,8 +3616,11 @@
       <c r="F37">
         <v>2019</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>105</v>
       </c>
@@ -3626,8 +3636,11 @@
       <c r="F38">
         <v>2020</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>105</v>
       </c>
@@ -3643,8 +3656,11 @@
       <c r="F39">
         <v>2021</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D40">
         <v>2025</v>
       </c>
@@ -3654,111 +3670,144 @@
       <c r="F40">
         <v>2022</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E41">
         <v>2027</v>
       </c>
       <c r="F41">
         <v>2023</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E42">
         <v>2030</v>
       </c>
       <c r="F42">
         <v>2024</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E43">
         <v>2033</v>
       </c>
       <c r="F43">
         <v>2025</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E44">
         <v>2035</v>
       </c>
       <c r="F44">
         <v>2026</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E45">
         <v>2037</v>
       </c>
       <c r="F45">
         <v>2027</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E46">
         <v>2040</v>
       </c>
       <c r="F46">
         <v>2028</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F47">
         <v>2029</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F48">
         <v>2030</v>
       </c>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F49">
         <v>2031</v>
       </c>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F50">
         <v>2032</v>
       </c>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F51">
         <v>2033</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F52">
         <v>2034</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F53">
         <v>2035</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F54">
         <v>2036</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F55">
         <v>2037</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F56">
         <v>2038</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F57">
         <v>2039</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F58">
         <v>2040</v>
       </c>
@@ -3776,7 +3825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3943,8 +3992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:G33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4001,7 +4050,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="9">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>